<commit_message>
Added and modified excel files. Added project files
</commit_message>
<xml_diff>
--- a/excel/Emergencyprocess_PHBT_splines.xlsx
+++ b/excel/Emergencyprocess_PHBT_splines.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projektit\whole_blood_research\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E960153-2665-4A95-999B-F071BE39F24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2A9BCF-7D51-4349-98BA-F59AB3313E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03F3FB12-313A-4338-B057-6B74AD45E5AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{03F3FB12-313A-4338-B057-6B74AD45E5AA}"/>
   </bookViews>
   <sheets>
     <sheet name="PHBT_transfused_noLTOWB" sheetId="1" r:id="rId1"/>
-    <sheet name="PHBT_transfused_LTOWB" sheetId="2" r:id="rId2"/>
-    <sheet name="possible_useful_articles" sheetId="3" r:id="rId3"/>
+    <sheet name="yritys" sheetId="5" r:id="rId2"/>
+    <sheet name="PHBT_transfused_LTOWB" sheetId="2" r:id="rId3"/>
+    <sheet name="possible_useful_articles" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>Article</t>
   </si>
@@ -200,6 +201,18 @@
   </si>
   <si>
     <t>Products transfused</t>
+  </si>
+  <si>
+    <t>mortality</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>(at least 3 units of the product)</t>
   </si>
 </sst>
 </file>
@@ -591,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042CC0A0-1190-4B1E-BAE6-A9A83887E41C}">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,11 +993,662 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB0492F-CAA5-4E98-8C38-3483F1AE953F}">
+  <dimension ref="A1:U43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="E3">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <f>30*24</f>
+        <v>720</v>
+      </c>
+      <c r="E4">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>720</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>720</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>13.3</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>26</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>18</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>720</v>
+      </c>
+      <c r="E21">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="7">
+        <v>6</v>
+      </c>
+      <c r="E23" s="7">
+        <v>16.8</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7">
+        <v>24</v>
+      </c>
+      <c r="E24" s="7">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="7">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="7">
+        <v>24</v>
+      </c>
+      <c r="E27" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="7">
+        <v>6</v>
+      </c>
+      <c r="E28" s="7">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="7">
+        <v>24</v>
+      </c>
+      <c r="E29" s="7">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="7">
+        <v>6</v>
+      </c>
+      <c r="E31" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="7">
+        <v>24</v>
+      </c>
+      <c r="E32" s="7">
+        <v>14.1</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="7">
+        <v>720</v>
+      </c>
+      <c r="E33" s="7">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="7">
+        <v>6</v>
+      </c>
+      <c r="E34" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="7">
+        <v>24</v>
+      </c>
+      <c r="E35" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="7">
+        <v>720</v>
+      </c>
+      <c r="E36" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{399B3D6C-13F6-43A8-8B7B-872B11446F5E}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{0F028F8E-4724-41F9-98B0-6586F79E52E1}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{BCCC9D10-90F2-488C-B3C9-A086BF6F7B11}"/>
+    <hyperlink ref="B14" r:id="rId4" xr:uid="{2BAE1989-6C46-4DB1-9DDA-2D100E4EBD15}"/>
+    <hyperlink ref="B19" r:id="rId5" xr:uid="{E47D32F8-2CA1-4EA3-B94C-7F21442AE074}"/>
+    <hyperlink ref="B23" r:id="rId6" xr:uid="{822EE903-5A35-43E1-86A1-0B4D6EE6AC43}"/>
+    <hyperlink ref="B26" r:id="rId7" xr:uid="{6DE98DE6-3C90-482C-8AFD-0BC948F31316}"/>
+    <hyperlink ref="B31" r:id="rId8" xr:uid="{F0E657F7-C1C1-4C4C-9B50-08A8C22F95AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB16E479-6047-42D0-885D-96D2640FFC84}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,7 +1827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2969613-2499-4E13-99E7-DBA0805B3122}">
   <dimension ref="A1:I6"/>
   <sheetViews>

</xml_diff>